<commit_message>
Update of sql and codebook to include patient_id + patient_program_id
</commit_message>
<xml_diff>
--- a/PK/tbemr_basicRegister_codebook_v1.5_pk.xlsx
+++ b/PK/tbemr_basicRegister_codebook_v1.5_pk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msfintl-my.sharepoint.com/personal/kristina_reinhardt_newyork_msf_org/Documents/github/mart-tbemr-query-library/PK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{3F628ECC-ADCD-4099-BEC7-9B7DA5B7586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6E02DCE-FF1F-48E4-8962-480BB6EE5C63}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{3F628ECC-ADCD-4099-BEC7-9B7DA5B7586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D2B3F35-7B5B-4ADB-97D1-6A94EC5C8434}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="query_changelog" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="313">
   <si>
     <t>Column</t>
   </si>
@@ -953,10 +953,38 @@
     <t>Added baseline assessment date/year/quarter for dashboard filtering.</t>
   </si>
   <si>
-    <t>Removed voided program enrollements</t>
-  </si>
-  <si>
     <t>patient_program_voided = false</t>
+  </si>
+  <si>
+    <t>99_patient_id</t>
+  </si>
+  <si>
+    <t>99_patietn_program_id</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>patient_program_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The patient_id is a background id number assigned in the OMRS database to identify data associated with a particular patient. This column can be used to connect data from other tables available in the analytics database with this register for further analysis in the tool. This column should be used when connecting additional demographic data to this register. Demographic data includes any data collected in the registration page of Bahmni. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The patient_program_id is a background id number assigned in the OMRS database to identify data associated with a particular patient program enrollment. This column can be used to connect data from other tables available in the analytics database with this register for further analysis in the tool. This column should be used when connecting additional data during care to this register. Additional data includes any data collected in the clinical module in Bahmni. </t>
+  </si>
+  <si>
+    <t>Removed voided program enrollements.</t>
+  </si>
+  <si>
+    <t>Add patient_id and patient_program_id columns to register to faciltate.
+Harmonization of query version with main query (all implementations to be on v1.6 of register)</t>
   </si>
 </sst>
 </file>
@@ -1252,12 +1280,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1284,13 +1312,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1636,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFB7678-3E18-497F-ABA7-7D2FE6D40AA7}">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,24 +1675,24 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>43521</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1781,7 +1806,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>44169</v>
       </c>
@@ -1792,56 +1817,62 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="2:4" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="20">
+    <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="19">
         <v>44739</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="2:4" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="20">
+    <row r="16" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="19">
         <v>44739</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="19">
         <v>44741</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="19">
         <v>44834</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>302</v>
-      </c>
-      <c r="D18" s="22" t="s">
+      <c r="C18" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="2:4" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="19">
+        <v>44935</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
@@ -1857,55 +1888,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CC844-63E2-4B85-BD9F-12E3C1EFFCA3}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46" style="11" customWidth="1"/>
-    <col min="2" max="2" width="33" style="11" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" style="11" customWidth="1"/>
-    <col min="4" max="6" width="27" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="11" customWidth="1"/>
-    <col min="8" max="9" width="23" style="11" customWidth="1"/>
-    <col min="10" max="10" width="49.109375" style="11" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="11"/>
+    <col min="1" max="1" width="46" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="27" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="23" style="1" customWidth="1"/>
+    <col min="10" max="10" width="49.109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="13" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1935,7 +1966,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
@@ -4006,61 +4037,119 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" s="2" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G71" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H73" s="2">
         <v>1</v>
       </c>
-      <c r="I71" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="I73" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="2" t="s">
+      <c r="C74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4072,6 +4161,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070CE95ABCCDF824688903FE290C52AA9" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="407cfcb431a1568ce500e5bc0124fa9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="500fc99d-b194-414e-9bc2-944fb4fc9ef3" xmlns:ns4="95809629-8651-4b51-a536-1331494a3072" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58b948c687cb66ba8472d9e221e8c138" ns3:_="" ns4:_="">
     <xsd:import namespace="500fc99d-b194-414e-9bc2-944fb4fc9ef3"/>
@@ -4280,22 +4384,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAC8D0C-DBC1-4884-B9C9-C3DF8114B459}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357647DF-603C-4CA9-B082-BB6ADB1E29DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EE0199-3B27-4E13-8063-710C7C97DB35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4312,21 +4418,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357647DF-603C-4CA9-B082-BB6ADB1E29DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAC8D0C-DBC1-4884-B9C9-C3DF8114B459}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>